<commit_message>
added more testing runs to the plots
</commit_message>
<xml_diff>
--- a/benchmarks/results/plots/results-TestsvsPlock.xlsx
+++ b/benchmarks/results/plots/results-TestsvsPlock.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I244"/>
+  <dimension ref="A1:I343"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8014,6 +8014,3075 @@
         <v>0.04837253180190042</v>
       </c>
     </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B245" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C245" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D245" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E245" t="n">
+        <v>1072793.095470052</v>
+      </c>
+      <c r="F245" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G245" t="n">
+        <v>56.68049267723759</v>
+      </c>
+      <c r="H245" t="n">
+        <v>2640.981414812572</v>
+      </c>
+      <c r="I245" t="n">
+        <v>0.05165412374064176</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B246" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C246" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D246" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E246" t="n">
+        <v>1178212.070169422</v>
+      </c>
+      <c r="F246" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G246" t="n">
+        <v>56.68410045000375</v>
+      </c>
+      <c r="H246" t="n">
+        <v>2417.163433815813</v>
+      </c>
+      <c r="I246" t="n">
+        <v>0.05208385519669351</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B247" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C247" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D247" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E247" t="n">
+        <v>1172010.954010635</v>
+      </c>
+      <c r="F247" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G247" t="n">
+        <v>56.68390104686695</v>
+      </c>
+      <c r="H247" t="n">
+        <v>2424.184287366098</v>
+      </c>
+      <c r="I247" t="n">
+        <v>0.05207036300450743</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B248" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C248" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D248" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E248" t="n">
+        <v>781340.6360070902</v>
+      </c>
+      <c r="F248" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G248" t="n">
+        <v>56.66539073758901</v>
+      </c>
+      <c r="H248" t="n">
+        <v>3586.763275745398</v>
+      </c>
+      <c r="I248" t="n">
+        <v>0.04983744483730167</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B249" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C249" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D249" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E249" t="n">
+        <v>942569.6561355372</v>
+      </c>
+      <c r="F249" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G249" t="n">
+        <v>56.67449418787358</v>
+      </c>
+      <c r="H249" t="n">
+        <v>2993.547237371521</v>
+      </c>
+      <c r="I249" t="n">
+        <v>0.05097654249276338</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B250" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C250" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D250" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E250" t="n">
+        <v>954971.8884531101</v>
+      </c>
+      <c r="F250" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G250" t="n">
+        <v>56.67507159022423</v>
+      </c>
+      <c r="H250" t="n">
+        <v>2955.220046466073</v>
+      </c>
+      <c r="I250" t="n">
+        <v>0.05105012745363718</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B251" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C251" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D251" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E251" t="n">
+        <v>1109999.792422771</v>
+      </c>
+      <c r="F251" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G251" t="n">
+        <v>56.68196107412088</v>
+      </c>
+      <c r="H251" t="n">
+        <v>2553.49588530755</v>
+      </c>
+      <c r="I251" t="n">
+        <v>0.0518222399689018</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B252" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C252" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D252" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E252" t="n">
+        <v>669720.5451489342</v>
+      </c>
+      <c r="F252" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G252" t="n">
+        <v>56.65837316718935</v>
+      </c>
+      <c r="H252" t="n">
+        <v>4137.208664488034</v>
+      </c>
+      <c r="I252" t="n">
+        <v>0.04878192422973256</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B253" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C253" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D253" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E253" t="n">
+        <v>1066591.979311266</v>
+      </c>
+      <c r="F253" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G253" t="n">
+        <v>56.68024142879938</v>
+      </c>
+      <c r="H253" t="n">
+        <v>2656.237800050656</v>
+      </c>
+      <c r="I253" t="n">
+        <v>0.05162480878770818</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B254" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C254" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D254" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E254" t="n">
+        <v>1054189.746993693</v>
+      </c>
+      <c r="F254" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G254" t="n">
+        <v>56.67973224525753</v>
+      </c>
+      <c r="H254" t="n">
+        <v>2687.340671586911</v>
+      </c>
+      <c r="I254" t="n">
+        <v>0.05156504830177741</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B255" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C255" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D255" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E255" t="n">
+        <v>917765.1915003917</v>
+      </c>
+      <c r="F255" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G255" t="n">
+        <v>56.67361906009078</v>
+      </c>
+      <c r="H255" t="n">
+        <v>3074.31262676658</v>
+      </c>
+      <c r="I255" t="n">
+        <v>0.05082231846862658</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B256" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C256" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D256" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E256" t="n">
+        <v>675921.6613077208</v>
+      </c>
+      <c r="F256" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G256" t="n">
+        <v>56.65876344062507</v>
+      </c>
+      <c r="H256" t="n">
+        <v>4102.924508474816</v>
+      </c>
+      <c r="I256" t="n">
+        <v>0.04884755559877484</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B257" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C257" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D257" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E257" t="n">
+        <v>905362.9591828187</v>
+      </c>
+      <c r="F257" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G257" t="n">
+        <v>56.67300666801709</v>
+      </c>
+      <c r="H257" t="n">
+        <v>3115.4547434807</v>
+      </c>
+      <c r="I257" t="n">
+        <v>0.05074333546601673</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B258" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C258" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D258" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E258" t="n">
+        <v>1091396.443946412</v>
+      </c>
+      <c r="F258" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G258" t="n">
+        <v>56.68124113631831</v>
+      </c>
+      <c r="H258" t="n">
+        <v>2596.488440837139</v>
+      </c>
+      <c r="I258" t="n">
+        <v>0.05173961673900639</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B259" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C259" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D259" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E259" t="n">
+        <v>861955.1460713138</v>
+      </c>
+      <c r="F259" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G259" t="n">
+        <v>56.67062599061922</v>
+      </c>
+      <c r="H259" t="n">
+        <v>3267.557709748629</v>
+      </c>
+      <c r="I259" t="n">
+        <v>0.05045097770986243</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B260" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C260" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D260" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E260" t="n">
+        <v>936368.5399767508</v>
+      </c>
+      <c r="F260" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G260" t="n">
+        <v>56.67405929626911</v>
+      </c>
+      <c r="H260" t="n">
+        <v>3013.721688961359</v>
+      </c>
+      <c r="I260" t="n">
+        <v>0.05093749982842249</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B261" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C261" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D261" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E261" t="n">
+        <v>768938.4036895173</v>
+      </c>
+      <c r="F261" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G261" t="n">
+        <v>56.66425303430641</v>
+      </c>
+      <c r="H261" t="n">
+        <v>3641.102858139988</v>
+      </c>
+      <c r="I261" t="n">
+        <v>0.04973255035664968</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B262" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C262" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D262" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E262" t="n">
+        <v>626312.7320374293</v>
+      </c>
+      <c r="F262" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G262" t="n">
+        <v>56.65532229713481</v>
+      </c>
+      <c r="H262" t="n">
+        <v>4391.914224581619</v>
+      </c>
+      <c r="I262" t="n">
+        <v>0.04829385294716138</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B263" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C263" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D263" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E263" t="n">
+        <v>1103798.676263984</v>
+      </c>
+      <c r="F263" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G263" t="n">
+        <v>56.68172323076406</v>
+      </c>
+      <c r="H263" t="n">
+        <v>2567.646670430119</v>
+      </c>
+      <c r="I263" t="n">
+        <v>0.05179504399913257</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B264" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C264" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D264" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E264" t="n">
+        <v>632513.8481962158</v>
+      </c>
+      <c r="F264" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G264" t="n">
+        <v>56.65565750664638</v>
+      </c>
+      <c r="H264" t="n">
+        <v>4353.855806272697</v>
+      </c>
+      <c r="I264" t="n">
+        <v>0.0483666115202265</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B265" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C265" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D265" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E265" t="n">
+        <v>992178.5854058288</v>
+      </c>
+      <c r="F265" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G265" t="n">
+        <v>56.6772204517948</v>
+      </c>
+      <c r="H265" t="n">
+        <v>2849.454335177881</v>
+      </c>
+      <c r="I265" t="n">
+        <v>0.05125394765882731</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B266" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C266" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D266" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E266" t="n">
+        <v>1153407.605534276</v>
+      </c>
+      <c r="F266" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G266" t="n">
+        <v>56.68317117937617</v>
+      </c>
+      <c r="H266" t="n">
+        <v>2462.09652049243</v>
+      </c>
+      <c r="I266" t="n">
+        <v>0.05199740420424755</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B267" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C267" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D267" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E267" t="n">
+        <v>948770.7722943235</v>
+      </c>
+      <c r="F267" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G267" t="n">
+        <v>56.67478406795208</v>
+      </c>
+      <c r="H267" t="n">
+        <v>2974.258440690549</v>
+      </c>
+      <c r="I267" t="n">
+        <v>0.05101357465021029</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B268" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C268" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D268" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E268" t="n">
+        <v>961173.0046118966</v>
+      </c>
+      <c r="F268" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G268" t="n">
+        <v>56.67573559703194</v>
+      </c>
+      <c r="H268" t="n">
+        <v>2937.573297700369</v>
+      </c>
+      <c r="I268" t="n">
+        <v>0.05108459222872141</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B269" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C269" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D269" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E269" t="n">
+        <v>1029385.282358547</v>
+      </c>
+      <c r="F269" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G269" t="n">
+        <v>56.67879830643131</v>
+      </c>
+      <c r="H269" t="n">
+        <v>2751.813183180004</v>
+      </c>
+      <c r="I269" t="n">
+        <v>0.05144129291948224</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B270" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C270" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D270" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E270" t="n">
+        <v>688323.8936252937</v>
+      </c>
+      <c r="F270" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G270" t="n">
+        <v>56.65944394853116</v>
+      </c>
+      <c r="H270" t="n">
+        <v>4035.306151950784</v>
+      </c>
+      <c r="I270" t="n">
+        <v>0.04897698999757925</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B271" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C271" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D271" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E271" t="n">
+        <v>868156.2622301002</v>
+      </c>
+      <c r="F271" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G271" t="n">
+        <v>56.6705550298608</v>
+      </c>
+      <c r="H271" t="n">
+        <v>3241.410258382828</v>
+      </c>
+      <c r="I271" t="n">
+        <v>0.05050052444958403</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B272" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C272" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D272" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E272" t="n">
+        <v>1078994.211628839</v>
+      </c>
+      <c r="F272" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G272" t="n">
+        <v>56.68074171425983</v>
+      </c>
+      <c r="H272" t="n">
+        <v>2625.917833200137</v>
+      </c>
+      <c r="I272" t="n">
+        <v>0.05168306926817517</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B273" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C273" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D273" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E273" t="n">
+        <v>967374.120770683</v>
+      </c>
+      <c r="F273" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G273" t="n">
+        <v>56.67591238954119</v>
+      </c>
+      <c r="H273" t="n">
+        <v>2918.764488521347</v>
+      </c>
+      <c r="I273" t="n">
+        <v>0.05112042210434328</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B274" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C274" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D274" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E274" t="n">
+        <v>979776.3530882559</v>
+      </c>
+      <c r="F274" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G274" t="n">
+        <v>56.67608763337426</v>
+      </c>
+      <c r="H274" t="n">
+        <v>2891.165325278943</v>
+      </c>
+      <c r="I274" t="n">
+        <v>0.05117294537509536</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B275" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C275" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D275" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E275" t="n">
+        <v>1010781.933882188</v>
+      </c>
+      <c r="F275" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G275" t="n">
+        <v>56.67771541702132</v>
+      </c>
+      <c r="H275" t="n">
+        <v>2802.454146166868</v>
+      </c>
+      <c r="I275" t="n">
+        <v>0.05134360089919509</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B276" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C276" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D276" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E276" t="n">
+        <v>923966.3076591779</v>
+      </c>
+      <c r="F276" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G276" t="n">
+        <v>56.67372882379519</v>
+      </c>
+      <c r="H276" t="n">
+        <v>3049.818155163679</v>
+      </c>
+      <c r="I276" t="n">
+        <v>0.05086867748430641</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B277" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C277" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D277" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E277" t="n">
+        <v>1023184.166199761</v>
+      </c>
+      <c r="F277" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G277" t="n">
+        <v>56.67825506213479</v>
+      </c>
+      <c r="H277" t="n">
+        <v>2768.558863955212</v>
+      </c>
+      <c r="I277" t="n">
+        <v>0.05140871274119792</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B278" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C278" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D278" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E278" t="n">
+        <v>700726.1259428666</v>
+      </c>
+      <c r="F278" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G278" t="n">
+        <v>56.66048631504079</v>
+      </c>
+      <c r="H278" t="n">
+        <v>3970.11960546915</v>
+      </c>
+      <c r="I278" t="n">
+        <v>0.04910230053072178</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B279" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C279" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D279" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E279" t="n">
+        <v>1184413.186328208</v>
+      </c>
+      <c r="F279" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G279" t="n">
+        <v>56.68425231918151</v>
+      </c>
+      <c r="H279" t="n">
+        <v>2404.739324975647</v>
+      </c>
+      <c r="I279" t="n">
+        <v>0.05210767813730683</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B280" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C280" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D280" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E280" t="n">
+        <v>849552.9137537408</v>
+      </c>
+      <c r="F280" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G280" t="n">
+        <v>56.66931784012294</v>
+      </c>
+      <c r="H280" t="n">
+        <v>3308.14722744577</v>
+      </c>
+      <c r="I280" t="n">
+        <v>0.05037209870694535</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B281" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C281" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D281" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E281" t="n">
+        <v>756536.1713719442</v>
+      </c>
+      <c r="F281" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G281" t="n">
+        <v>56.66354552571458</v>
+      </c>
+      <c r="H281" t="n">
+        <v>3697.166530294654</v>
+      </c>
+      <c r="I281" t="n">
+        <v>0.04962506682121812</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B282" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C282" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D282" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E282" t="n">
+        <v>812346.2168010224</v>
+      </c>
+      <c r="F282" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G282" t="n">
+        <v>56.66734819694985</v>
+      </c>
+      <c r="H282" t="n">
+        <v>3456.080579681085</v>
+      </c>
+      <c r="I282" t="n">
+        <v>0.05008832494771949</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B283" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C283" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D283" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E283" t="n">
+        <v>1035586.398517334</v>
+      </c>
+      <c r="F283" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G283" t="n">
+        <v>56.67895706245374</v>
+      </c>
+      <c r="H283" t="n">
+        <v>2735.702502070864</v>
+      </c>
+      <c r="I283" t="n">
+        <v>0.05147211944004597</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B284" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C284" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D284" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E284" t="n">
+        <v>787541.7521658764</v>
+      </c>
+      <c r="F284" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G284" t="n">
+        <v>56.66574084723335</v>
+      </c>
+      <c r="H284" t="n">
+        <v>3560.003458535251</v>
+      </c>
+      <c r="I284" t="n">
+        <v>0.04988875944469699</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B285" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C285" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D285" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E285" t="n">
+        <v>985977.4692470422</v>
+      </c>
+      <c r="F285" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G285" t="n">
+        <v>56.67636562516513</v>
+      </c>
+      <c r="H285" t="n">
+        <v>2873.077183495716</v>
+      </c>
+      <c r="I285" t="n">
+        <v>0.05120768028404287</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B286" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C286" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D286" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E286" t="n">
+        <v>1203016.534804567</v>
+      </c>
+      <c r="F286" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G286" t="n">
+        <v>56.68477089931686</v>
+      </c>
+      <c r="H286" t="n">
+        <v>2368.331043072458</v>
+      </c>
+      <c r="I286" t="n">
+        <v>0.05217743978705382</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B287" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C287" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D287" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E287" t="n">
+        <v>1047988.630834906</v>
+      </c>
+      <c r="F287" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G287" t="n">
+        <v>56.67946754673265</v>
+      </c>
+      <c r="H287" t="n">
+        <v>2703.150764410212</v>
+      </c>
+      <c r="I287" t="n">
+        <v>0.0515346586482671</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B288" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C288" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D288" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E288" t="n">
+        <v>1122402.024740344</v>
+      </c>
+      <c r="F288" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G288" t="n">
+        <v>56.68209245645519</v>
+      </c>
+      <c r="H288" t="n">
+        <v>2523.194175767794</v>
+      </c>
+      <c r="I288" t="n">
+        <v>0.05187989001463664</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B289" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C289" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D289" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E289" t="n">
+        <v>1085195.327787625</v>
+      </c>
+      <c r="F289" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G289" t="n">
+        <v>56.6809968574137</v>
+      </c>
+      <c r="H289" t="n">
+        <v>2611.184858067354</v>
+      </c>
+      <c r="I289" t="n">
+        <v>0.05171137508051973</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B290" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C290" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D290" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E290" t="n">
+        <v>762737.2875307308</v>
+      </c>
+      <c r="F290" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G290" t="n">
+        <v>56.66390362719024</v>
+      </c>
+      <c r="H290" t="n">
+        <v>3668.938525434899</v>
+      </c>
+      <c r="I290" t="n">
+        <v>0.04967918416420861</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B291" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C291" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D291" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E291" t="n">
+        <v>1227820.999439713</v>
+      </c>
+      <c r="F291" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G291" t="n">
+        <v>56.68558988243593</v>
+      </c>
+      <c r="H291" t="n">
+        <v>2322.016523561291</v>
+      </c>
+      <c r="I291" t="n">
+        <v>0.05226649054608069</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B292" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C292" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D292" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E292" t="n">
+        <v>744133.9390543716</v>
+      </c>
+      <c r="F292" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G292" t="n">
+        <v>56.66282982592257</v>
+      </c>
+      <c r="H292" t="n">
+        <v>3754.829515559863</v>
+      </c>
+      <c r="I292" t="n">
+        <v>0.0495145312257048</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B293" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C293" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D293" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E293" t="n">
+        <v>793742.8683246629</v>
+      </c>
+      <c r="F293" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G293" t="n">
+        <v>56.66632816319424</v>
+      </c>
+      <c r="H293" t="n">
+        <v>3532.068917545515</v>
+      </c>
+      <c r="I293" t="n">
+        <v>0.04994265624808597</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B294" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C294" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D294" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E294" t="n">
+        <v>737932.8228955851</v>
+      </c>
+      <c r="F294" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G294" t="n">
+        <v>56.66246898848611</v>
+      </c>
+      <c r="H294" t="n">
+        <v>3784.276670334546</v>
+      </c>
+      <c r="I294" t="n">
+        <v>0.0494580887339874</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B295" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C295" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D295" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E295" t="n">
+        <v>1134804.257057917</v>
+      </c>
+      <c r="F295" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G295" t="n">
+        <v>56.68238340553353</v>
+      </c>
+      <c r="H295" t="n">
+        <v>2501.276528956058</v>
+      </c>
+      <c r="I295" t="n">
+        <v>0.05192188924701584</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B296" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C296" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D296" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E296" t="n">
+        <v>1097597.560105198</v>
+      </c>
+      <c r="F296" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G296" t="n">
+        <v>56.68153528832146</v>
+      </c>
+      <c r="H296" t="n">
+        <v>2582.044909705169</v>
+      </c>
+      <c r="I296" t="n">
+        <v>0.05176745651366862</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B297" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C297" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D297" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E297" t="n">
+        <v>855754.0299125273</v>
+      </c>
+      <c r="F297" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G297" t="n">
+        <v>56.67030308083989</v>
+      </c>
+      <c r="H297" t="n">
+        <v>3290.704574803025</v>
+      </c>
+      <c r="I297" t="n">
+        <v>0.05040656659972227</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B298" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C298" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D298" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E298" t="n">
+        <v>719329.4744192258</v>
+      </c>
+      <c r="F298" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G298" t="n">
+        <v>56.66133572797417</v>
+      </c>
+      <c r="H298" t="n">
+        <v>3875.10032599379</v>
+      </c>
+      <c r="I298" t="n">
+        <v>0.04928400787613663</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B299" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C299" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D299" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E299" t="n">
+        <v>1128603.14089913</v>
+      </c>
+      <c r="F299" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G299" t="n">
+        <v>56.68232255949815</v>
+      </c>
+      <c r="H299" t="n">
+        <v>2509.609067224411</v>
+      </c>
+      <c r="I299" t="n">
+        <v>0.05190600067603433</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B300" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C300" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D300" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E300" t="n">
+        <v>1190614.302486994</v>
+      </c>
+      <c r="F300" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G300" t="n">
+        <v>56.68433471382376</v>
+      </c>
+      <c r="H300" t="n">
+        <v>2392.334616893283</v>
+      </c>
+      <c r="I300" t="n">
+        <v>0.05213127778598332</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B301" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C301" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D301" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E301" t="n">
+        <v>1141005.373216703</v>
+      </c>
+      <c r="F301" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G301" t="n">
+        <v>56.682677108292</v>
+      </c>
+      <c r="H301" t="n">
+        <v>2487.953471930761</v>
+      </c>
+      <c r="I301" t="n">
+        <v>0.05194761202886361</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B302" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C302" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D302" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E302" t="n">
+        <v>663519.4289901479</v>
+      </c>
+      <c r="F302" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G302" t="n">
+        <v>56.65799141210717</v>
+      </c>
+      <c r="H302" t="n">
+        <v>4172.113490539857</v>
+      </c>
+      <c r="I302" t="n">
+        <v>0.04871507604884587</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B303" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C303" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D303" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E303" t="n">
+        <v>1209217.650963354</v>
+      </c>
+      <c r="F303" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G303" t="n">
+        <v>56.6849784106948</v>
+      </c>
+      <c r="H303" t="n">
+        <v>2356.544681262053</v>
+      </c>
+      <c r="I303" t="n">
+        <v>0.05220010094841927</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B304" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C304" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D304" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E304" t="n">
+        <v>874357.3783888866</v>
+      </c>
+      <c r="F304" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G304" t="n">
+        <v>56.67152232288163</v>
+      </c>
+      <c r="H304" t="n">
+        <v>3221.064642318628</v>
+      </c>
+      <c r="I304" t="n">
+        <v>0.05054057511612236</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B305" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C305" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D305" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E305" t="n">
+        <v>880558.494547673</v>
+      </c>
+      <c r="F305" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G305" t="n">
+        <v>56.67188190252937</v>
+      </c>
+      <c r="H305" t="n">
+        <v>3198.847829108341</v>
+      </c>
+      <c r="I305" t="n">
+        <v>0.05058325082885651</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B306" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C306" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D306" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E306" t="n">
+        <v>682122.7774665073</v>
+      </c>
+      <c r="F306" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G306" t="n">
+        <v>56.65914173655499</v>
+      </c>
+      <c r="H306" t="n">
+        <v>4068.975861527711</v>
+      </c>
+      <c r="I306" t="n">
+        <v>0.0489125814432865</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B307" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C307" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D307" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E307" t="n">
+        <v>620111.615878643</v>
+      </c>
+      <c r="F307" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G307" t="n">
+        <v>56.65519792301154</v>
+      </c>
+      <c r="H307" t="n">
+        <v>4430.595581919822</v>
+      </c>
+      <c r="I307" t="n">
+        <v>0.04822012939658356</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B308" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C308" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D308" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E308" t="n">
+        <v>644916.0805137887</v>
+      </c>
+      <c r="F308" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G308" t="n">
+        <v>56.65649596484396</v>
+      </c>
+      <c r="H308" t="n">
+        <v>4279.484381171912</v>
+      </c>
+      <c r="I308" t="n">
+        <v>0.04850905829854518</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B309" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C309" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D309" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E309" t="n">
+        <v>1041787.51467612</v>
+      </c>
+      <c r="F309" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G309" t="n">
+        <v>56.67921913781323</v>
+      </c>
+      <c r="H309" t="n">
+        <v>2719.427169049934</v>
+      </c>
+      <c r="I309" t="n">
+        <v>0.05150338611741596</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B310" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C310" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D310" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E310" t="n">
+        <v>694525.0097840801</v>
+      </c>
+      <c r="F310" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G310" t="n">
+        <v>56.66011395466933</v>
+      </c>
+      <c r="H310" t="n">
+        <v>4002.690567050909</v>
+      </c>
+      <c r="I310" t="n">
+        <v>0.04903990272286379</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B311" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C311" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D311" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E311" t="n">
+        <v>799943.9844834494</v>
+      </c>
+      <c r="F311" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G311" t="n">
+        <v>56.66625609063962</v>
+      </c>
+      <c r="H311" t="n">
+        <v>3505.930924571194</v>
+      </c>
+      <c r="I311" t="n">
+        <v>0.04999210382704296</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B312" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C312" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D312" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E312" t="n">
+        <v>930167.4238179644</v>
+      </c>
+      <c r="F312" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G312" t="n">
+        <v>56.67335107307855</v>
+      </c>
+      <c r="H312" t="n">
+        <v>3033.577823137894</v>
+      </c>
+      <c r="I312" t="n">
+        <v>0.05089885509875607</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B313" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C313" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D313" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E313" t="n">
+        <v>1215418.76712214</v>
+      </c>
+      <c r="F313" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G313" t="n">
+        <v>56.68518406835047</v>
+      </c>
+      <c r="H313" t="n">
+        <v>2344.898143557535</v>
+      </c>
+      <c r="I313" t="n">
+        <v>0.0522224939078268</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B314" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C314" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D314" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E314" t="n">
+        <v>818547.3329598086</v>
+      </c>
+      <c r="F314" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G314" t="n">
+        <v>56.66773356580151</v>
+      </c>
+      <c r="H314" t="n">
+        <v>3430.921206099822</v>
+      </c>
+      <c r="I314" t="n">
+        <v>0.05013662818934533</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B315" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C315" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D315" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E315" t="n">
+        <v>731731.7067367986</v>
+      </c>
+      <c r="F315" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G315" t="n">
+        <v>56.66202346445814</v>
+      </c>
+      <c r="H315" t="n">
+        <v>3814.075554591312</v>
+      </c>
+      <c r="I315" t="n">
+        <v>0.04940089765149461</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B316" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C316" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D316" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E316" t="n">
+        <v>1221619.883280927</v>
+      </c>
+      <c r="F316" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G316" t="n">
+        <v>56.68538788726404</v>
+      </c>
+      <c r="H316" t="n">
+        <v>2333.389417822866</v>
+      </c>
+      <c r="I316" t="n">
+        <v>0.05224462251164786</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B317" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C317" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D317" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E317" t="n">
+        <v>1196815.418645781</v>
+      </c>
+      <c r="F317" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G317" t="n">
+        <v>56.6845460700529</v>
+      </c>
+      <c r="H317" t="n">
+        <v>2380.261942061697</v>
+      </c>
+      <c r="I317" t="n">
+        <v>0.05215448814956149</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B318" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C318" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D318" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E318" t="n">
+        <v>725530.5905780124</v>
+      </c>
+      <c r="F318" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G318" t="n">
+        <v>56.66170317181162</v>
+      </c>
+      <c r="H318" t="n">
+        <v>3844.400151840449</v>
+      </c>
+      <c r="I318" t="n">
+        <v>0.04934284144935765</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B319" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C319" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D319" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E319" t="n">
+        <v>706927.2421016529</v>
+      </c>
+      <c r="F319" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G319" t="n">
+        <v>56.66085701176659</v>
+      </c>
+      <c r="H319" t="n">
+        <v>3938.010113116669</v>
+      </c>
+      <c r="I319" t="n">
+        <v>0.04916381857568702</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B320" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C320" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D320" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E320" t="n">
+        <v>973575.2369294695</v>
+      </c>
+      <c r="F320" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G320" t="n">
+        <v>56.67616087074545</v>
+      </c>
+      <c r="H320" t="n">
+        <v>2900.283713788272</v>
+      </c>
+      <c r="I320" t="n">
+        <v>0.05115588666221926</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B321" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C321" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D321" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E321" t="n">
+        <v>1004580.817723401</v>
+      </c>
+      <c r="F321" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G321" t="n">
+        <v>56.67782699653186</v>
+      </c>
+      <c r="H321" t="n">
+        <v>2814.747864955866</v>
+      </c>
+      <c r="I321" t="n">
+        <v>0.05132054359429333</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B322" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C322" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D322" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E322" t="n">
+        <v>1147206.48937549</v>
+      </c>
+      <c r="F322" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G322" t="n">
+        <v>56.68290063859148</v>
+      </c>
+      <c r="H322" t="n">
+        <v>2474.839093053104</v>
+      </c>
+      <c r="I322" t="n">
+        <v>0.05197281896796588</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B323" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C323" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D323" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E323" t="n">
+        <v>1060390.86315248</v>
+      </c>
+      <c r="F323" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G323" t="n">
+        <v>56.67998795577275</v>
+      </c>
+      <c r="H323" t="n">
+        <v>2671.689899888269</v>
+      </c>
+      <c r="I323" t="n">
+        <v>0.0515951188553376</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B324" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C324" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D324" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E324" t="n">
+        <v>837150.6814361679</v>
+      </c>
+      <c r="F324" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G324" t="n">
+        <v>56.66869655067428</v>
+      </c>
+      <c r="H324" t="n">
+        <v>3356.906346503915</v>
+      </c>
+      <c r="I324" t="n">
+        <v>0.05027865222253077</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B325" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C325" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D325" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E325" t="n">
+        <v>886759.6107064595</v>
+      </c>
+      <c r="F325" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G325" t="n">
+        <v>56.67206975965276</v>
+      </c>
+      <c r="H325" t="n">
+        <v>3179.291615132578</v>
+      </c>
+      <c r="I325" t="n">
+        <v>0.05062079895551815</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B326" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C326" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D326" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E326" t="n">
+        <v>998379.7015646149</v>
+      </c>
+      <c r="F326" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G326" t="n">
+        <v>56.6774677307554</v>
+      </c>
+      <c r="H326" t="n">
+        <v>2831.965290598342</v>
+      </c>
+      <c r="I326" t="n">
+        <v>0.05128737627508681</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B327" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C327" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D327" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E327" t="n">
+        <v>1016983.050040975</v>
+      </c>
+      <c r="F327" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G327" t="n">
+        <v>56.67798638299627</v>
+      </c>
+      <c r="H327" t="n">
+        <v>2785.395174180874</v>
+      </c>
+      <c r="I327" t="n">
+        <v>0.05137636991583319</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B328" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C328" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D328" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E328" t="n">
+        <v>1159608.721693062</v>
+      </c>
+      <c r="F328" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G328" t="n">
+        <v>56.6833907921217</v>
+      </c>
+      <c r="H328" t="n">
+        <v>2449.268215504868</v>
+      </c>
+      <c r="I328" t="n">
+        <v>0.0520220617837083</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B329" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C329" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D329" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E329" t="n">
+        <v>899161.8430240322</v>
+      </c>
+      <c r="F329" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G329" t="n">
+        <v>56.67269680864766</v>
+      </c>
+      <c r="H329" t="n">
+        <v>3136.44643573069</v>
+      </c>
+      <c r="I329" t="n">
+        <v>0.05070303938677372</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B330" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C330" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D330" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E330" t="n">
+        <v>830949.5652773816</v>
+      </c>
+      <c r="F330" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G330" t="n">
+        <v>56.66792064045012</v>
+      </c>
+      <c r="H330" t="n">
+        <v>3381.517888505954</v>
+      </c>
+      <c r="I330" t="n">
+        <v>0.05023074068590787</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B331" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C331" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D331" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E331" t="n">
+        <v>775139.5198483038</v>
+      </c>
+      <c r="F331" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G331" t="n">
+        <v>56.66460683882693</v>
+      </c>
+      <c r="H331" t="n">
+        <v>3613.655720843717</v>
+      </c>
+      <c r="I331" t="n">
+        <v>0.04978517723477051</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B332" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C332" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D332" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E332" t="n">
+        <v>1116200.908581557</v>
+      </c>
+      <c r="F332" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G332" t="n">
+        <v>56.6818602863573</v>
+      </c>
+      <c r="H332" t="n">
+        <v>2536.951607116792</v>
+      </c>
+      <c r="I332" t="n">
+        <v>0.05185344913590852</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B333" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C333" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D333" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E333" t="n">
+        <v>1165809.837851849</v>
+      </c>
+      <c r="F333" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G333" t="n">
+        <v>56.68368634814443</v>
+      </c>
+      <c r="H333" t="n">
+        <v>2436.704740125633</v>
+      </c>
+      <c r="I333" t="n">
+        <v>0.05204629675983713</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B334" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C334" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D334" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E334" t="n">
+        <v>657318.3128313615</v>
+      </c>
+      <c r="F334" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G334" t="n">
+        <v>56.6574701898281</v>
+      </c>
+      <c r="H334" t="n">
+        <v>4207.403072223454</v>
+      </c>
+      <c r="I334" t="n">
+        <v>0.04864736890561248</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B335" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C335" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D335" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E335" t="n">
+        <v>843351.7975949544</v>
+      </c>
+      <c r="F335" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G335" t="n">
+        <v>56.66902534443408</v>
+      </c>
+      <c r="H335" t="n">
+        <v>3333.081160937221</v>
+      </c>
+      <c r="I335" t="n">
+        <v>0.0503243609717219</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B336" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C336" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D336" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E336" t="n">
+        <v>824748.4491185951</v>
+      </c>
+      <c r="F336" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G336" t="n">
+        <v>56.66758769817457</v>
+      </c>
+      <c r="H336" t="n">
+        <v>3405.945475402889</v>
+      </c>
+      <c r="I336" t="n">
+        <v>0.05018388045372196</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B337" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C337" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D337" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E337" t="n">
+        <v>651117.1966725751</v>
+      </c>
+      <c r="F337" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G337" t="n">
+        <v>56.65688506675941</v>
+      </c>
+      <c r="H337" t="n">
+        <v>4243.081531815159</v>
+      </c>
+      <c r="I337" t="n">
+        <v>0.04857876353665505</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B338" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C338" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D338" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E338" t="n">
+        <v>892960.7268652457</v>
+      </c>
+      <c r="F338" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G338" t="n">
+        <v>56.67238450578943</v>
+      </c>
+      <c r="H338" t="n">
+        <v>3157.723900864348</v>
+      </c>
+      <c r="I338" t="n">
+        <v>0.05066219672156049</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B339" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C339" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D339" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E339" t="n">
+        <v>638714.9643550023</v>
+      </c>
+      <c r="F339" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G339" t="n">
+        <v>56.65610576262713</v>
+      </c>
+      <c r="H339" t="n">
+        <v>4316.415709938902</v>
+      </c>
+      <c r="I339" t="n">
+        <v>0.0484383466138946</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B340" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C340" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D340" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E340" t="n">
+        <v>806145.1006422358</v>
+      </c>
+      <c r="F340" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G340" t="n">
+        <v>56.6670073579557</v>
+      </c>
+      <c r="H340" t="n">
+        <v>3481.620620425673</v>
+      </c>
+      <c r="I340" t="n">
+        <v>0.05003933894465223</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B341" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C341" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D341" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E341" t="n">
+        <v>911564.0753416051</v>
+      </c>
+      <c r="F341" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G341" t="n">
+        <v>56.67331408462382</v>
+      </c>
+      <c r="H341" t="n">
+        <v>3094.744417864298</v>
+      </c>
+      <c r="I341" t="n">
+        <v>0.05078309334219451</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B342" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C342" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D342" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E342" t="n">
+        <v>713128.3582604394</v>
+      </c>
+      <c r="F342" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G342" t="n">
+        <v>56.66098680566832</v>
+      </c>
+      <c r="H342" t="n">
+        <v>3906.451490101829</v>
+      </c>
+      <c r="I342" t="n">
+        <v>0.04922395314224801</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=full_open_targetGroups=False_targetAct=False_targetTests=True_optimizeLockdowns=False</t>
+        </is>
+      </c>
+      <c r="B343" t="n">
+        <v>1859951.5</v>
+      </c>
+      <c r="C343" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D343" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E343" t="n">
+        <v>750335.055213158</v>
+      </c>
+      <c r="F343" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G343" t="n">
+        <v>56.66318868344793</v>
+      </c>
+      <c r="H343" t="n">
+        <v>3725.794949061199</v>
+      </c>
+      <c r="I343" t="n">
+        <v>0.04957018651993803</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>